<commit_message>
GPLIM-6233 add NovaSeq SP and fix name used for external library and walkup flowcell
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZFailTest2.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZFailTest2.xlsx
@@ -345,9 +345,6 @@
     <t>Lib-MOCK.FSK1.A</t>
   </si>
   <si>
-    <t>NovaSeq</t>
-  </si>
-  <si>
     <t>Sample No.</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>NovaSeq SP</t>
   </si>
 </sst>
 </file>
@@ -1275,13 +1275,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="8" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="8" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="161">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
@@ -1845,8 +1845,8 @@
   </sheetPr>
   <dimension ref="A2:AL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W25" workbookViewId="0">
-      <selection activeCell="AE30" sqref="AE30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1956,8 +1956,8 @@
       <c r="I5" s="3"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -1976,8 +1976,8 @@
       <c r="J6" s="14"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="29" spans="1:38" s="29" customFormat="1" ht="64" customHeight="1">
       <c r="A29" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>17</v>
@@ -2412,696 +2412,696 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="47" customFormat="1">
-      <c r="A30" s="46">
+    <row r="30" spans="1:38" s="46" customFormat="1">
+      <c r="A30" s="45">
         <v>22</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="46">
         <v>963357</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="L30" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="M30" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="N30" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="O30" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="P30" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q30" s="46">
+        <v>12345</v>
+      </c>
+      <c r="R30" s="45">
+        <v>0</v>
+      </c>
+      <c r="S30" s="45">
+        <v>419</v>
+      </c>
+      <c r="T30" s="46">
+        <v>123</v>
+      </c>
+      <c r="U30" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="V30" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="W30" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="X30" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y30" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z30" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA30" s="45">
+        <v>96</v>
+      </c>
+      <c r="AB30" s="45">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC30" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD30" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE30" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF30" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG30" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI30" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ30" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK30" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL30" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" s="46" customFormat="1">
+      <c r="A31" s="45">
+        <v>22</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="46">
+        <v>963357</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="G30" s="47" t="s">
+      <c r="G31" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="H30" s="47" t="s">
+      <c r="H31" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="I31" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="47" t="s">
+      <c r="J31" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="K30" s="46" t="s">
+      <c r="K31" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="L30" s="46" t="s">
+      <c r="L31" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="M30" s="48" t="s">
+      <c r="M31" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="N30" s="47" t="s">
+      <c r="N31" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="O30" s="47" t="s">
+      <c r="O31" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="P31" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q31" s="46">
+        <v>12345</v>
+      </c>
+      <c r="R31" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="S31" s="45">
+        <v>419</v>
+      </c>
+      <c r="T31" s="46">
+        <v>123</v>
+      </c>
+      <c r="U31" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="V31" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="W31" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="X31" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y31" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z31" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA31" s="45">
+        <v>96</v>
+      </c>
+      <c r="AB31" s="45">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC31" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD31" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE31" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF31" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG31" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI31" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ31" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK31" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL31" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" s="46" customFormat="1">
+      <c r="A32" s="45">
+        <v>22</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="46">
+        <v>963357</v>
+      </c>
+      <c r="E32" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="J32" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="K32" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="M32" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="N32" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="P32" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q32" s="46">
+        <v>12345</v>
+      </c>
+      <c r="R32" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="S32" s="45">
+        <v>419</v>
+      </c>
+      <c r="T32" s="46">
+        <v>123</v>
+      </c>
+      <c r="U32" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="V32" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="W32" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="X32" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y32" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z32" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA32" s="45">
+        <v>96</v>
+      </c>
+      <c r="AB32" s="45">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC32" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD32" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE32" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF32" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG32" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI32" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ32" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK32" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL32" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" s="46" customFormat="1">
+      <c r="A33" s="45">
+        <v>22</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="46">
+        <v>963357</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H33" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I33" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="L33" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="M33" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="N33" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="O33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="P30" s="47" t="s">
+      <c r="P33" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="Q30" s="47">
+      <c r="Q33" s="46">
         <v>12345</v>
       </c>
-      <c r="R30" s="46">
-        <v>0</v>
-      </c>
-      <c r="S30" s="46">
+      <c r="R33" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="S33" s="45">
         <v>419</v>
       </c>
-      <c r="T30" s="47">
+      <c r="T33" s="46">
         <v>123</v>
       </c>
-      <c r="U30" s="46" t="s">
+      <c r="U33" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="V30" s="47" t="s">
+      <c r="V33" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="W30" s="47">
+      <c r="W33" s="46">
         <v>123456789</v>
       </c>
-      <c r="X30" s="47" t="s">
+      <c r="X33" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="Y30" s="46" t="s">
+      <c r="Y33" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="Z30" s="46" t="s">
+      <c r="Z33" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="AA30" s="46">
+      <c r="AA33" s="45">
         <v>96</v>
       </c>
-      <c r="AB30" s="46">
+      <c r="AB33" s="45">
         <v>7.4000000953674316</v>
       </c>
-      <c r="AC30" s="46" t="s">
+      <c r="AC33" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="46" t="s">
+      <c r="AD33" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="AE30" s="46" t="s">
+      <c r="AE33" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="AF30" s="49" t="s">
+      <c r="AF33" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="AG30" s="47">
+      <c r="AG33" s="46">
         <v>1</v>
       </c>
-      <c r="AH30" s="47" t="s">
+      <c r="AH33" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="AI30" s="46" t="s">
+      <c r="AI33" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="AJ30" s="47" t="s">
+      <c r="AJ33" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="AK30" s="47" t="s">
+      <c r="AK33" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="AL30" s="46" t="s">
+      <c r="AL33" s="45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:38" s="47" customFormat="1">
-      <c r="A31" s="46">
+    <row r="34" spans="1:38" s="46" customFormat="1">
+      <c r="A34" s="45">
         <v>22</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B34" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C34" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="47">
+      <c r="D34" s="46">
         <v>963357</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E34" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="47" t="s">
+      <c r="F34" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="G34" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="H31" s="47" t="s">
+      <c r="H34" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="I31" s="47" t="s">
+      <c r="I34" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="J31" s="47" t="s">
+      <c r="J34" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="K31" s="46" t="s">
+      <c r="K34" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="L31" s="46" t="s">
+      <c r="L34" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="M31" s="48" t="s">
+      <c r="M34" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="N31" s="47" t="s">
+      <c r="N34" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="O31" s="47" t="s">
+      <c r="O34" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q34" s="46">
+        <v>12345</v>
+      </c>
+      <c r="R34" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="S34" s="45">
+        <v>419</v>
+      </c>
+      <c r="T34" s="46">
+        <v>123</v>
+      </c>
+      <c r="U34" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="V34" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="W34" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="X34" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y34" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z34" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA34" s="45">
+        <v>96</v>
+      </c>
+      <c r="AB34" s="45">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC34" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD34" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE34" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF34" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG34" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH34" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI34" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ34" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK34" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL34" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" s="46" customFormat="1">
+      <c r="A35" s="45">
+        <v>22</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="46">
+        <v>963357</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="P31" s="47" t="s">
+      <c r="G35" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I35" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="L35" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="M35" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="N35" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="O35" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="P35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="Q31" s="47">
+      <c r="Q35" s="46">
         <v>12345</v>
       </c>
-      <c r="R31" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="S31" s="46">
+      <c r="R35" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="S35" s="45">
         <v>419</v>
       </c>
-      <c r="T31" s="47">
+      <c r="T35" s="46">
         <v>123</v>
       </c>
-      <c r="U31" s="46" t="s">
+      <c r="U35" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="V31" s="47" t="s">
+      <c r="V35" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="W31" s="47">
+      <c r="W35" s="46">
         <v>123456789</v>
       </c>
-      <c r="X31" s="47" t="s">
+      <c r="X35" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="Y31" s="46" t="s">
+      <c r="Y35" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="Z31" s="46" t="s">
+      <c r="Z35" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="AA31" s="46">
+      <c r="AA35" s="45">
         <v>96</v>
       </c>
-      <c r="AB31" s="46">
+      <c r="AB35" s="45">
         <v>7.4000000953674316</v>
       </c>
-      <c r="AC31" s="46" t="s">
+      <c r="AC35" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="AD31" s="46" t="s">
+      <c r="AD35" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="AE31" s="46" t="s">
+      <c r="AE35" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="AF31" s="49" t="s">
+      <c r="AF35" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="AG31" s="47">
+      <c r="AG35" s="46">
         <v>1</v>
       </c>
-      <c r="AH31" s="47" t="s">
+      <c r="AH35" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="AI31" s="46" t="s">
+      <c r="AI35" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="AJ31" s="47" t="s">
+      <c r="AJ35" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="AK31" s="47" t="s">
+      <c r="AK35" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="AL31" s="46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" s="47" customFormat="1">
-      <c r="A32" s="46">
-        <v>22</v>
-      </c>
-      <c r="B32" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="47">
-        <v>963357</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="G32" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H32" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="I32" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="J32" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="K32" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="L32" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="M32" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="N32" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="P32" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q32" s="47">
-        <v>12345</v>
-      </c>
-      <c r="R32" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="S32" s="46">
-        <v>419</v>
-      </c>
-      <c r="T32" s="47">
-        <v>123</v>
-      </c>
-      <c r="U32" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="V32" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="W32" s="47">
-        <v>123456789</v>
-      </c>
-      <c r="X32" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y32" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z32" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA32" s="46">
-        <v>96</v>
-      </c>
-      <c r="AB32" s="46">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC32" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD32" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE32" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF32" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG32" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI32" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ32" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK32" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL32" s="46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" s="47" customFormat="1">
-      <c r="A33" s="46">
-        <v>22</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="47">
-        <v>963357</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="G33" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H33" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="I33" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="J33" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="K33" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="L33" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="M33" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="N33" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="O33" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="P33" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q33" s="47">
-        <v>12345</v>
-      </c>
-      <c r="R33" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="S33" s="46">
-        <v>419</v>
-      </c>
-      <c r="T33" s="47">
-        <v>123</v>
-      </c>
-      <c r="U33" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="V33" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="W33" s="47">
-        <v>123456789</v>
-      </c>
-      <c r="X33" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y33" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z33" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA33" s="46">
-        <v>96</v>
-      </c>
-      <c r="AB33" s="46">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC33" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD33" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE33" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF33" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG33" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI33" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ33" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK33" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL33" s="46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38" s="47" customFormat="1">
-      <c r="A34" s="46">
-        <v>22</v>
-      </c>
-      <c r="B34" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="47">
-        <v>963357</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="I34" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="J34" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="K34" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="L34" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="M34" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="N34" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="O34" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="P34" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q34" s="47">
-        <v>12345</v>
-      </c>
-      <c r="R34" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="S34" s="46">
-        <v>419</v>
-      </c>
-      <c r="T34" s="47">
-        <v>123</v>
-      </c>
-      <c r="U34" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="V34" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="W34" s="47">
-        <v>123456789</v>
-      </c>
-      <c r="X34" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y34" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z34" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA34" s="46">
-        <v>96</v>
-      </c>
-      <c r="AB34" s="46">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC34" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD34" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE34" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF34" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG34" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI34" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ34" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK34" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL34" s="46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38" s="47" customFormat="1">
-      <c r="A35" s="46">
-        <v>22</v>
-      </c>
-      <c r="B35" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="47">
-        <v>963357</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="I35" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="J35" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="K35" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="L35" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="M35" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="N35" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="O35" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="P35" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q35" s="47">
-        <v>12345</v>
-      </c>
-      <c r="R35" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="S35" s="46">
-        <v>419</v>
-      </c>
-      <c r="T35" s="47">
-        <v>123</v>
-      </c>
-      <c r="U35" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="V35" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="W35" s="47">
-        <v>123456789</v>
-      </c>
-      <c r="X35" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y35" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z35" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA35" s="46">
-        <v>96</v>
-      </c>
-      <c r="AB35" s="46">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC35" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD35" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE35" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF35" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG35" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH35" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI35" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ35" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK35" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL35" s="46" t="s">
+      <c r="AL35" s="45" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>